<commit_message>
4/27 first success getting knowing object's height.
</commit_message>
<xml_diff>
--- a/point_cloud.xlsx
+++ b/point_cloud.xlsx
@@ -354,20 +354,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C103"/>
+  <dimension ref="A1:C287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+    <sheetView tabSelected="1" topLeftCell="A274" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E284" sqref="E284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1">
-        <v>573</v>
+        <v>1017</v>
       </c>
       <c r="B1">
-        <v>507</v>
+        <v>0</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -375,10 +375,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>573</v>
+        <v>1017</v>
       </c>
       <c r="B2">
-        <v>508</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -386,10 +386,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>573</v>
+        <v>1017</v>
       </c>
       <c r="B3">
-        <v>524</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -397,10 +397,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>573</v>
+        <v>1017</v>
       </c>
       <c r="B4">
-        <v>525</v>
+        <v>30</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -408,10 +408,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>573</v>
+        <v>1017</v>
       </c>
       <c r="B5">
-        <v>526</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -419,10 +419,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>575</v>
+        <v>1018</v>
       </c>
       <c r="B6">
-        <v>198</v>
+        <v>50</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -430,10 +430,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>575</v>
+        <v>1017</v>
       </c>
       <c r="B7">
-        <v>199</v>
+        <v>60</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -441,10 +441,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>575</v>
+        <v>1018</v>
       </c>
       <c r="B8">
-        <v>200</v>
+        <v>70</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -452,10 +452,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>575</v>
+        <v>1018</v>
       </c>
       <c r="B9">
-        <v>201</v>
+        <v>80</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -463,10 +463,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>575</v>
+        <v>1018</v>
       </c>
       <c r="B10">
-        <v>202</v>
+        <v>90</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -474,10 +474,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>575</v>
+        <v>1018</v>
       </c>
       <c r="B11">
-        <v>203</v>
+        <v>100</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -485,10 +485,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>575</v>
+        <v>1018</v>
       </c>
       <c r="B12">
-        <v>204</v>
+        <v>110</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -496,10 +496,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>575</v>
+        <v>1018</v>
       </c>
       <c r="B13">
-        <v>205</v>
+        <v>120</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -507,10 +507,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>575</v>
+        <v>1018</v>
       </c>
       <c r="B14">
-        <v>206</v>
+        <v>130</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -518,10 +518,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>575</v>
+        <v>1018</v>
       </c>
       <c r="B15">
-        <v>207</v>
+        <v>140</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -529,10 +529,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>574</v>
+        <v>1018</v>
       </c>
       <c r="B16">
-        <v>208</v>
+        <v>150</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -540,10 +540,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>575</v>
+        <v>1018</v>
       </c>
       <c r="B17">
-        <v>209</v>
+        <v>160</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -551,948 +551,2972 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>686</v>
+        <v>1018</v>
       </c>
       <c r="B18">
-        <v>525</v>
+        <v>170</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>686</v>
+        <v>1019</v>
       </c>
       <c r="B19">
-        <v>526</v>
+        <v>180</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>686</v>
+        <v>1019</v>
       </c>
       <c r="B20">
-        <v>527</v>
+        <v>190</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>686</v>
+        <v>1019</v>
       </c>
       <c r="B21">
-        <v>528</v>
+        <v>200</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>686</v>
+        <v>1019</v>
       </c>
       <c r="B22">
-        <v>529</v>
+        <v>210</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>690</v>
+        <v>1019</v>
       </c>
       <c r="B23">
-        <v>540</v>
+        <v>220</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>690</v>
+        <v>1019</v>
       </c>
       <c r="B24">
-        <v>541</v>
+        <v>230</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>690</v>
+        <v>1019</v>
       </c>
       <c r="B25">
-        <v>542</v>
+        <v>240</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>755</v>
+        <v>1019</v>
       </c>
       <c r="B26">
-        <v>820</v>
+        <v>250</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>755</v>
+        <v>1019</v>
       </c>
       <c r="B27">
-        <v>821</v>
+        <v>260</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>756</v>
+        <v>1019</v>
       </c>
       <c r="B28">
-        <v>822</v>
+        <v>270</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>757</v>
+        <v>1019</v>
       </c>
       <c r="B29">
-        <v>823</v>
+        <v>280</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>760</v>
+        <v>1020</v>
       </c>
       <c r="B30">
-        <v>840</v>
+        <v>290</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>760</v>
+        <v>1019</v>
       </c>
       <c r="B31">
-        <v>841</v>
+        <v>300</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>760</v>
+        <v>1019</v>
       </c>
       <c r="B32">
-        <v>842</v>
+        <v>310</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>760</v>
+        <v>1020</v>
       </c>
       <c r="B33">
-        <v>843</v>
+        <v>320</v>
       </c>
       <c r="C33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>760</v>
+        <v>1019</v>
       </c>
       <c r="B34">
-        <v>844</v>
+        <v>330</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>621</v>
+        <v>1020</v>
       </c>
       <c r="B35">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>622</v>
+        <v>1019</v>
       </c>
       <c r="B36">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>622</v>
+        <v>1020</v>
       </c>
       <c r="B37">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="C37">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>622</v>
+        <v>1020</v>
       </c>
       <c r="B38">
-        <v>353</v>
+        <v>370</v>
       </c>
       <c r="C38">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>623</v>
+        <v>1020</v>
       </c>
       <c r="B39">
-        <v>354</v>
+        <v>380</v>
       </c>
       <c r="C39">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>623</v>
+        <v>1020</v>
       </c>
       <c r="B40">
-        <v>355</v>
+        <v>390</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>624</v>
+        <v>1019</v>
       </c>
       <c r="B41">
-        <v>356</v>
+        <v>400</v>
       </c>
       <c r="C41">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>653</v>
+        <v>1020</v>
       </c>
       <c r="B42">
-        <v>424</v>
+        <v>410</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>654</v>
+        <v>1020</v>
       </c>
       <c r="B43">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="C43">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>654</v>
+        <v>1020</v>
       </c>
       <c r="B44">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
-        <v>654</v>
+        <v>1020</v>
       </c>
       <c r="B45">
-        <v>427</v>
+        <v>440</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46">
-        <v>655</v>
+        <v>1020</v>
       </c>
       <c r="B46">
-        <v>428</v>
+        <v>450</v>
       </c>
       <c r="C46">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>656</v>
+        <v>1020</v>
       </c>
       <c r="B47">
-        <v>429</v>
+        <v>460</v>
       </c>
       <c r="C47">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>678</v>
+        <v>1020</v>
       </c>
       <c r="B48">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="C48">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49">
-        <v>678</v>
+        <v>1019</v>
       </c>
       <c r="B49">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C49">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>679</v>
+        <v>1020</v>
       </c>
       <c r="B50">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="C50">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>680</v>
+        <v>1019</v>
       </c>
       <c r="B51">
-        <v>485</v>
+        <v>500</v>
       </c>
       <c r="C51">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52">
-        <v>679</v>
+        <v>1020</v>
       </c>
       <c r="B52">
-        <v>486</v>
+        <v>510</v>
       </c>
       <c r="C52">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53">
-        <v>680</v>
+        <v>1021</v>
       </c>
       <c r="B53">
-        <v>487</v>
+        <v>520</v>
       </c>
       <c r="C53">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54">
-        <v>790</v>
+        <v>1021</v>
       </c>
       <c r="B54">
-        <v>754</v>
+        <v>530</v>
       </c>
       <c r="C54">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55">
-        <v>790</v>
+        <v>1020</v>
       </c>
       <c r="B55">
-        <v>755</v>
+        <v>540</v>
       </c>
       <c r="C55">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56">
-        <v>791</v>
+        <v>1020</v>
       </c>
       <c r="B56">
-        <v>756</v>
+        <v>550</v>
       </c>
       <c r="C56">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
-        <v>792</v>
+        <v>1021</v>
       </c>
       <c r="B57">
-        <v>757</v>
+        <v>560</v>
       </c>
       <c r="C57">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
-        <v>792</v>
+        <v>1021</v>
       </c>
       <c r="B58">
-        <v>758</v>
+        <v>570</v>
       </c>
       <c r="C58">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59">
-        <v>792</v>
+        <v>1021</v>
       </c>
       <c r="B59">
-        <v>759</v>
+        <v>580</v>
       </c>
       <c r="C59">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60">
-        <v>792</v>
+        <v>1021</v>
       </c>
       <c r="B60">
-        <v>760</v>
+        <v>590</v>
       </c>
       <c r="C60">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61">
-        <v>570</v>
+        <v>1021</v>
       </c>
       <c r="B61">
-        <v>418</v>
+        <v>600</v>
       </c>
       <c r="C61">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62">
-        <v>570</v>
+        <v>1021</v>
       </c>
       <c r="B62">
-        <v>419</v>
+        <v>610</v>
       </c>
       <c r="C62">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63">
-        <v>570</v>
+        <v>1021</v>
       </c>
       <c r="B63">
-        <v>420</v>
+        <v>620</v>
       </c>
       <c r="C63">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64">
-        <v>570</v>
+        <v>1021</v>
       </c>
       <c r="B64">
-        <v>421</v>
+        <v>630</v>
       </c>
       <c r="C64">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65">
-        <v>570</v>
+        <v>1021</v>
       </c>
       <c r="B65">
-        <v>422</v>
+        <v>640</v>
       </c>
       <c r="C65">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66">
-        <v>569</v>
+        <v>1021</v>
       </c>
       <c r="B66">
-        <v>423</v>
+        <v>650</v>
       </c>
       <c r="C66">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67">
-        <v>569</v>
+        <v>1021</v>
       </c>
       <c r="B67">
-        <v>424</v>
+        <v>660</v>
       </c>
       <c r="C67">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68">
-        <v>570</v>
+        <v>1021</v>
       </c>
       <c r="B68">
-        <v>425</v>
+        <v>670</v>
       </c>
       <c r="C68">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69">
-        <v>583</v>
+        <v>1021</v>
       </c>
       <c r="B69">
-        <v>632</v>
+        <v>680</v>
       </c>
       <c r="C69">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70">
-        <v>583</v>
+        <v>1021</v>
       </c>
       <c r="B70">
-        <v>633</v>
+        <v>690</v>
       </c>
       <c r="C70">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71">
-        <v>583</v>
+        <v>1022</v>
       </c>
       <c r="B71">
-        <v>634</v>
+        <v>700</v>
       </c>
       <c r="C71">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72">
-        <v>584</v>
+        <v>1021</v>
       </c>
       <c r="B72">
-        <v>635</v>
+        <v>710</v>
       </c>
       <c r="C72">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73">
-        <v>583</v>
+        <v>1021</v>
       </c>
       <c r="B73">
-        <v>636</v>
+        <v>720</v>
       </c>
       <c r="C73">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74">
-        <v>583</v>
+        <v>1021</v>
       </c>
       <c r="B74">
-        <v>637</v>
+        <v>730</v>
       </c>
       <c r="C74">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75">
-        <v>595</v>
+        <v>1022</v>
       </c>
       <c r="B75">
-        <v>875</v>
+        <v>740</v>
       </c>
       <c r="C75">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76">
-        <v>595</v>
+        <v>1021</v>
       </c>
       <c r="B76">
-        <v>876</v>
+        <v>750</v>
       </c>
       <c r="C76">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77">
-        <v>595</v>
+        <v>1021</v>
       </c>
       <c r="B77">
-        <v>877</v>
+        <v>760</v>
       </c>
       <c r="C77">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78">
-        <v>595</v>
+        <v>1022</v>
       </c>
       <c r="B78">
-        <v>878</v>
+        <v>770</v>
       </c>
       <c r="C78">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79">
-        <v>595</v>
+        <v>1021</v>
       </c>
       <c r="B79">
-        <v>879</v>
+        <v>780</v>
       </c>
       <c r="C79">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80">
-        <v>595</v>
+        <v>1021</v>
       </c>
       <c r="B80">
-        <v>880</v>
+        <v>790</v>
       </c>
       <c r="C80">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81">
-        <v>594</v>
+        <v>1022</v>
       </c>
       <c r="B81">
-        <v>881</v>
+        <v>800</v>
       </c>
       <c r="C81">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82">
-        <v>608</v>
+        <v>1022</v>
       </c>
       <c r="B82">
-        <v>338</v>
+        <v>810</v>
       </c>
       <c r="C82">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83">
-        <v>608</v>
+        <v>1021</v>
       </c>
       <c r="B83">
-        <v>339</v>
+        <v>820</v>
       </c>
       <c r="C83">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84">
-        <v>609</v>
+        <v>1021</v>
       </c>
       <c r="B84">
-        <v>340</v>
+        <v>830</v>
       </c>
       <c r="C84">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85">
-        <v>609</v>
+        <v>1022</v>
       </c>
       <c r="B85">
-        <v>341</v>
+        <v>840</v>
       </c>
       <c r="C85">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86">
-        <v>609</v>
+        <v>1021</v>
       </c>
       <c r="B86">
-        <v>342</v>
+        <v>850</v>
       </c>
       <c r="C86">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87">
-        <v>609</v>
+        <v>1022</v>
       </c>
       <c r="B87">
-        <v>343</v>
+        <v>860</v>
       </c>
       <c r="C87">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88">
-        <v>592</v>
+        <v>1022</v>
       </c>
       <c r="B88">
-        <v>233</v>
+        <v>870</v>
       </c>
       <c r="C88">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89">
-        <v>592</v>
+        <v>1022</v>
       </c>
       <c r="B89">
-        <v>234</v>
+        <v>880</v>
       </c>
       <c r="C89">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90">
-        <v>592</v>
+        <v>1023</v>
       </c>
       <c r="B90">
-        <v>235</v>
+        <v>890</v>
       </c>
       <c r="C90">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91">
-        <v>593</v>
+        <v>1023</v>
       </c>
       <c r="B91">
-        <v>236</v>
+        <v>900</v>
       </c>
       <c r="C91">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92">
-        <v>593</v>
+        <v>1022</v>
       </c>
       <c r="B92">
-        <v>237</v>
+        <v>910</v>
       </c>
       <c r="C92">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93">
-        <v>593</v>
+        <v>1022</v>
       </c>
       <c r="B93">
-        <v>238</v>
+        <v>920</v>
       </c>
       <c r="C93">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94">
-        <v>593</v>
+        <v>1023</v>
       </c>
       <c r="B94">
-        <v>239</v>
+        <v>930</v>
       </c>
       <c r="C94">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95">
-        <v>646</v>
+        <v>1023</v>
       </c>
       <c r="B95">
-        <v>602</v>
+        <v>940</v>
       </c>
       <c r="C95">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96">
-        <v>647</v>
+        <v>1023</v>
       </c>
       <c r="B96">
-        <v>603</v>
+        <v>950</v>
       </c>
       <c r="C96">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97">
-        <v>647</v>
+        <v>1023</v>
       </c>
       <c r="B97">
-        <v>604</v>
+        <v>960</v>
       </c>
       <c r="C97">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98">
-        <v>647</v>
+        <v>1025</v>
       </c>
       <c r="B98">
-        <v>605</v>
+        <v>0</v>
       </c>
       <c r="C98">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99">
-        <v>647</v>
+        <v>1024</v>
       </c>
       <c r="B99">
-        <v>606</v>
+        <v>10</v>
       </c>
       <c r="C99">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100">
-        <v>646</v>
+        <v>1023</v>
       </c>
       <c r="B100">
-        <v>607</v>
+        <v>20</v>
       </c>
       <c r="C100">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101">
-        <v>646</v>
+        <v>1021</v>
       </c>
       <c r="B101">
-        <v>608</v>
+        <v>30</v>
       </c>
       <c r="C101">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102">
-        <v>647</v>
+        <v>1020</v>
       </c>
       <c r="B102">
-        <v>609</v>
+        <v>40</v>
       </c>
       <c r="C102">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103">
-        <v>646</v>
+        <v>1019</v>
       </c>
       <c r="B103">
+        <v>50</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104">
+        <v>1018</v>
+      </c>
+      <c r="B104">
+        <v>60</v>
+      </c>
+      <c r="C104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105">
+        <v>1017</v>
+      </c>
+      <c r="B105">
+        <v>70</v>
+      </c>
+      <c r="C105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106">
+        <v>1016</v>
+      </c>
+      <c r="B106">
+        <v>80</v>
+      </c>
+      <c r="C106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107">
+        <v>1015</v>
+      </c>
+      <c r="B107">
+        <v>90</v>
+      </c>
+      <c r="C107">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108">
+        <v>1014</v>
+      </c>
+      <c r="B108">
+        <v>100</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109">
+        <v>1013</v>
+      </c>
+      <c r="B109">
+        <v>110</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110">
+        <v>1012</v>
+      </c>
+      <c r="B110">
+        <v>120</v>
+      </c>
+      <c r="C110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111">
+        <v>1010</v>
+      </c>
+      <c r="B111">
+        <v>130</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112">
+        <v>1010</v>
+      </c>
+      <c r="B112">
+        <v>140</v>
+      </c>
+      <c r="C112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113">
+        <v>1008</v>
+      </c>
+      <c r="B113">
+        <v>150</v>
+      </c>
+      <c r="C113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114">
+        <v>1007</v>
+      </c>
+      <c r="B114">
+        <v>160</v>
+      </c>
+      <c r="C114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115">
+        <v>1007</v>
+      </c>
+      <c r="B115">
+        <v>170</v>
+      </c>
+      <c r="C115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116">
+        <v>1006</v>
+      </c>
+      <c r="B116">
+        <v>180</v>
+      </c>
+      <c r="C116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117">
+        <v>1004</v>
+      </c>
+      <c r="B117">
+        <v>190</v>
+      </c>
+      <c r="C117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118">
+        <v>1004</v>
+      </c>
+      <c r="B118">
+        <v>200</v>
+      </c>
+      <c r="C118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119">
+        <v>1002</v>
+      </c>
+      <c r="B119">
+        <v>220</v>
+      </c>
+      <c r="C119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120">
+        <v>999</v>
+      </c>
+      <c r="B120">
+        <v>240</v>
+      </c>
+      <c r="C120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121">
+        <v>998</v>
+      </c>
+      <c r="B121">
+        <v>250</v>
+      </c>
+      <c r="C121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122">
+        <v>996</v>
+      </c>
+      <c r="B122">
+        <v>260</v>
+      </c>
+      <c r="C122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123">
+        <v>995</v>
+      </c>
+      <c r="B123">
+        <v>270</v>
+      </c>
+      <c r="C123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124">
+        <v>994</v>
+      </c>
+      <c r="B124">
+        <v>280</v>
+      </c>
+      <c r="C124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125">
+        <v>993</v>
+      </c>
+      <c r="B125">
+        <v>290</v>
+      </c>
+      <c r="C125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126">
+        <v>991</v>
+      </c>
+      <c r="B126">
+        <v>300</v>
+      </c>
+      <c r="C126">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127">
+        <v>990</v>
+      </c>
+      <c r="B127">
+        <v>310</v>
+      </c>
+      <c r="C127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128">
+        <v>990</v>
+      </c>
+      <c r="B128">
+        <v>320</v>
+      </c>
+      <c r="C128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129">
+        <v>989</v>
+      </c>
+      <c r="B129">
+        <v>330</v>
+      </c>
+      <c r="C129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130">
+        <v>987</v>
+      </c>
+      <c r="B130">
+        <v>340</v>
+      </c>
+      <c r="C130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131">
+        <v>987</v>
+      </c>
+      <c r="B131">
+        <v>350</v>
+      </c>
+      <c r="C131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132">
+        <v>985</v>
+      </c>
+      <c r="B132">
+        <v>360</v>
+      </c>
+      <c r="C132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133">
+        <v>984</v>
+      </c>
+      <c r="B133">
+        <v>370</v>
+      </c>
+      <c r="C133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134">
+        <v>983</v>
+      </c>
+      <c r="B134">
+        <v>380</v>
+      </c>
+      <c r="C134">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135">
+        <v>981</v>
+      </c>
+      <c r="B135">
+        <v>390</v>
+      </c>
+      <c r="C135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136">
+        <v>980</v>
+      </c>
+      <c r="B136">
+        <v>400</v>
+      </c>
+      <c r="C136">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137">
+        <v>980</v>
+      </c>
+      <c r="B137">
+        <v>410</v>
+      </c>
+      <c r="C137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138">
+        <v>979</v>
+      </c>
+      <c r="B138">
+        <v>420</v>
+      </c>
+      <c r="C138">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139">
+        <v>978</v>
+      </c>
+      <c r="B139">
+        <v>430</v>
+      </c>
+      <c r="C139">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140">
+        <v>976</v>
+      </c>
+      <c r="B140">
+        <v>440</v>
+      </c>
+      <c r="C140">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141">
+        <v>975</v>
+      </c>
+      <c r="B141">
+        <v>450</v>
+      </c>
+      <c r="C141">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142">
+        <v>975</v>
+      </c>
+      <c r="B142">
+        <v>460</v>
+      </c>
+      <c r="C142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143">
+        <v>973</v>
+      </c>
+      <c r="B143">
+        <v>470</v>
+      </c>
+      <c r="C143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144">
+        <v>972</v>
+      </c>
+      <c r="B144">
+        <v>480</v>
+      </c>
+      <c r="C144">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145">
+        <v>972</v>
+      </c>
+      <c r="B145">
+        <v>490</v>
+      </c>
+      <c r="C145">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146">
+        <v>969</v>
+      </c>
+      <c r="B146">
+        <v>500</v>
+      </c>
+      <c r="C146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147">
+        <v>968</v>
+      </c>
+      <c r="B147">
+        <v>510</v>
+      </c>
+      <c r="C147">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148">
+        <v>968</v>
+      </c>
+      <c r="B148">
+        <v>520</v>
+      </c>
+      <c r="C148">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149">
+        <v>966</v>
+      </c>
+      <c r="B149">
+        <v>530</v>
+      </c>
+      <c r="C149">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150">
+        <v>965</v>
+      </c>
+      <c r="B150">
+        <v>540</v>
+      </c>
+      <c r="C150">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151">
+        <v>963</v>
+      </c>
+      <c r="B151">
+        <v>550</v>
+      </c>
+      <c r="C151">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152">
+        <v>963</v>
+      </c>
+      <c r="B152">
+        <v>560</v>
+      </c>
+      <c r="C152">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153">
+        <v>962</v>
+      </c>
+      <c r="B153">
+        <v>570</v>
+      </c>
+      <c r="C153">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154">
+        <v>960</v>
+      </c>
+      <c r="B154">
+        <v>580</v>
+      </c>
+      <c r="C154">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155">
+        <v>959</v>
+      </c>
+      <c r="B155">
+        <v>590</v>
+      </c>
+      <c r="C155">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156">
+        <v>959</v>
+      </c>
+      <c r="B156">
+        <v>600</v>
+      </c>
+      <c r="C156">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157">
+        <v>957</v>
+      </c>
+      <c r="B157">
         <v>610</v>
       </c>
-      <c r="C103">
-        <v>5</v>
+      <c r="C157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158">
+        <v>956</v>
+      </c>
+      <c r="B158">
+        <v>620</v>
+      </c>
+      <c r="C158">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159">
+        <v>955</v>
+      </c>
+      <c r="B159">
+        <v>630</v>
+      </c>
+      <c r="C159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160">
+        <v>954</v>
+      </c>
+      <c r="B160">
+        <v>640</v>
+      </c>
+      <c r="C160">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161">
+        <v>953</v>
+      </c>
+      <c r="B161">
+        <v>650</v>
+      </c>
+      <c r="C161">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162">
+        <v>952</v>
+      </c>
+      <c r="B162">
+        <v>660</v>
+      </c>
+      <c r="C162">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163">
+        <v>951</v>
+      </c>
+      <c r="B163">
+        <v>670</v>
+      </c>
+      <c r="C163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164">
+        <v>949</v>
+      </c>
+      <c r="B164">
+        <v>680</v>
+      </c>
+      <c r="C164">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165">
+        <v>949</v>
+      </c>
+      <c r="B165">
+        <v>690</v>
+      </c>
+      <c r="C165">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166">
+        <v>947</v>
+      </c>
+      <c r="B166">
+        <v>700</v>
+      </c>
+      <c r="C166">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167">
+        <v>946</v>
+      </c>
+      <c r="B167">
+        <v>710</v>
+      </c>
+      <c r="C167">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168">
+        <v>945</v>
+      </c>
+      <c r="B168">
+        <v>720</v>
+      </c>
+      <c r="C168">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169">
+        <v>944</v>
+      </c>
+      <c r="B169">
+        <v>730</v>
+      </c>
+      <c r="C169">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170">
+        <v>944</v>
+      </c>
+      <c r="B170">
+        <v>740</v>
+      </c>
+      <c r="C170">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171">
+        <v>941</v>
+      </c>
+      <c r="B171">
+        <v>750</v>
+      </c>
+      <c r="C171">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172">
+        <v>940</v>
+      </c>
+      <c r="B172">
+        <v>760</v>
+      </c>
+      <c r="C172">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173">
+        <v>939</v>
+      </c>
+      <c r="B173">
+        <v>770</v>
+      </c>
+      <c r="C173">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174">
+        <v>937</v>
+      </c>
+      <c r="B174">
+        <v>780</v>
+      </c>
+      <c r="C174">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175">
+        <v>937</v>
+      </c>
+      <c r="B175">
+        <v>790</v>
+      </c>
+      <c r="C175">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176">
+        <v>936</v>
+      </c>
+      <c r="B176">
+        <v>800</v>
+      </c>
+      <c r="C176">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177">
+        <v>934</v>
+      </c>
+      <c r="B177">
+        <v>810</v>
+      </c>
+      <c r="C177">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178">
+        <v>933</v>
+      </c>
+      <c r="B178">
+        <v>820</v>
+      </c>
+      <c r="C178">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179">
+        <v>933</v>
+      </c>
+      <c r="B179">
+        <v>830</v>
+      </c>
+      <c r="C179">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180">
+        <v>928</v>
+      </c>
+      <c r="B180">
+        <v>860</v>
+      </c>
+      <c r="C180">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181">
+        <v>928</v>
+      </c>
+      <c r="B181">
+        <v>870</v>
+      </c>
+      <c r="C181">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182">
+        <v>927</v>
+      </c>
+      <c r="B182">
+        <v>880</v>
+      </c>
+      <c r="C182">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183">
+        <v>926</v>
+      </c>
+      <c r="B183">
+        <v>890</v>
+      </c>
+      <c r="C183">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184">
+        <v>925</v>
+      </c>
+      <c r="B184">
+        <v>900</v>
+      </c>
+      <c r="C184">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185">
+        <v>924</v>
+      </c>
+      <c r="B185">
+        <v>910</v>
+      </c>
+      <c r="C185">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186">
+        <v>923</v>
+      </c>
+      <c r="B186">
+        <v>920</v>
+      </c>
+      <c r="C186">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187">
+        <v>921</v>
+      </c>
+      <c r="B187">
+        <v>930</v>
+      </c>
+      <c r="C187">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188">
+        <v>921</v>
+      </c>
+      <c r="B188">
+        <v>940</v>
+      </c>
+      <c r="C188">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189">
+        <v>920</v>
+      </c>
+      <c r="B189">
+        <v>950</v>
+      </c>
+      <c r="C189">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190">
+        <v>919</v>
+      </c>
+      <c r="B190">
+        <v>960</v>
+      </c>
+      <c r="C190">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191">
+        <v>953</v>
+      </c>
+      <c r="B191">
+        <v>0</v>
+      </c>
+      <c r="C191">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192">
+        <v>953</v>
+      </c>
+      <c r="B192">
+        <v>10</v>
+      </c>
+      <c r="C192">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193">
+        <v>952</v>
+      </c>
+      <c r="B193">
+        <v>20</v>
+      </c>
+      <c r="C193">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194">
+        <v>953</v>
+      </c>
+      <c r="B194">
+        <v>30</v>
+      </c>
+      <c r="C194">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195">
+        <v>953</v>
+      </c>
+      <c r="B195">
+        <v>40</v>
+      </c>
+      <c r="C195">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196">
+        <v>953</v>
+      </c>
+      <c r="B196">
+        <v>50</v>
+      </c>
+      <c r="C196">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197">
+        <v>953</v>
+      </c>
+      <c r="B197">
+        <v>60</v>
+      </c>
+      <c r="C197">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198">
+        <v>953</v>
+      </c>
+      <c r="B198">
+        <v>70</v>
+      </c>
+      <c r="C198">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199">
+        <v>952</v>
+      </c>
+      <c r="B199">
+        <v>80</v>
+      </c>
+      <c r="C199">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200">
+        <v>953</v>
+      </c>
+      <c r="B200">
+        <v>90</v>
+      </c>
+      <c r="C200">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201">
+        <v>952</v>
+      </c>
+      <c r="B201">
+        <v>100</v>
+      </c>
+      <c r="C201">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202">
+        <v>953</v>
+      </c>
+      <c r="B202">
+        <v>110</v>
+      </c>
+      <c r="C202">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203">
+        <v>953</v>
+      </c>
+      <c r="B203">
+        <v>120</v>
+      </c>
+      <c r="C203">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204">
+        <v>953</v>
+      </c>
+      <c r="B204">
+        <v>130</v>
+      </c>
+      <c r="C204">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205">
+        <v>952</v>
+      </c>
+      <c r="B205">
+        <v>140</v>
+      </c>
+      <c r="C205">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206">
+        <v>952</v>
+      </c>
+      <c r="B206">
+        <v>150</v>
+      </c>
+      <c r="C206">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207">
+        <v>953</v>
+      </c>
+      <c r="B207">
+        <v>160</v>
+      </c>
+      <c r="C207">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208">
+        <v>953</v>
+      </c>
+      <c r="B208">
+        <v>170</v>
+      </c>
+      <c r="C208">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209">
+        <v>952</v>
+      </c>
+      <c r="B209">
+        <v>180</v>
+      </c>
+      <c r="C209">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210">
+        <v>953</v>
+      </c>
+      <c r="B210">
+        <v>190</v>
+      </c>
+      <c r="C210">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211">
+        <v>952</v>
+      </c>
+      <c r="B211">
+        <v>200</v>
+      </c>
+      <c r="C211">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212">
+        <v>953</v>
+      </c>
+      <c r="B212">
+        <v>210</v>
+      </c>
+      <c r="C212">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213">
+        <v>953</v>
+      </c>
+      <c r="B213">
+        <v>220</v>
+      </c>
+      <c r="C213">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214">
+        <v>952</v>
+      </c>
+      <c r="B214">
+        <v>230</v>
+      </c>
+      <c r="C214">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215">
+        <v>952</v>
+      </c>
+      <c r="B215">
+        <v>240</v>
+      </c>
+      <c r="C215">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216">
+        <v>952</v>
+      </c>
+      <c r="B216">
+        <v>250</v>
+      </c>
+      <c r="C216">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217">
+        <v>952</v>
+      </c>
+      <c r="B217">
+        <v>260</v>
+      </c>
+      <c r="C217">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218">
+        <v>953</v>
+      </c>
+      <c r="B218">
+        <v>270</v>
+      </c>
+      <c r="C218">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219">
+        <v>952</v>
+      </c>
+      <c r="B219">
+        <v>280</v>
+      </c>
+      <c r="C219">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220">
+        <v>952</v>
+      </c>
+      <c r="B220">
+        <v>290</v>
+      </c>
+      <c r="C220">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221">
+        <v>952</v>
+      </c>
+      <c r="B221">
+        <v>300</v>
+      </c>
+      <c r="C221">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222">
+        <v>952</v>
+      </c>
+      <c r="B222">
+        <v>310</v>
+      </c>
+      <c r="C222">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223">
+        <v>952</v>
+      </c>
+      <c r="B223">
+        <v>320</v>
+      </c>
+      <c r="C223">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224">
+        <v>952</v>
+      </c>
+      <c r="B224">
+        <v>330</v>
+      </c>
+      <c r="C224">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3">
+      <c r="A225">
+        <v>952</v>
+      </c>
+      <c r="B225">
+        <v>340</v>
+      </c>
+      <c r="C225">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226">
+        <v>951</v>
+      </c>
+      <c r="B226">
+        <v>350</v>
+      </c>
+      <c r="C226">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3">
+      <c r="A227">
+        <v>952</v>
+      </c>
+      <c r="B227">
+        <v>360</v>
+      </c>
+      <c r="C227">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
+      <c r="A228">
+        <v>952</v>
+      </c>
+      <c r="B228">
+        <v>370</v>
+      </c>
+      <c r="C228">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3">
+      <c r="A229">
+        <v>952</v>
+      </c>
+      <c r="B229">
+        <v>380</v>
+      </c>
+      <c r="C229">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
+      <c r="A230">
+        <v>951</v>
+      </c>
+      <c r="B230">
+        <v>390</v>
+      </c>
+      <c r="C230">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231">
+        <v>952</v>
+      </c>
+      <c r="B231">
+        <v>400</v>
+      </c>
+      <c r="C231">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232">
+        <v>951</v>
+      </c>
+      <c r="B232">
+        <v>410</v>
+      </c>
+      <c r="C232">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233">
+        <v>952</v>
+      </c>
+      <c r="B233">
+        <v>420</v>
+      </c>
+      <c r="C233">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3">
+      <c r="A234">
+        <v>951</v>
+      </c>
+      <c r="B234">
+        <v>430</v>
+      </c>
+      <c r="C234">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3">
+      <c r="A235">
+        <v>951</v>
+      </c>
+      <c r="B235">
+        <v>440</v>
+      </c>
+      <c r="C235">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236">
+        <v>952</v>
+      </c>
+      <c r="B236">
+        <v>450</v>
+      </c>
+      <c r="C236">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3">
+      <c r="A237">
+        <v>952</v>
+      </c>
+      <c r="B237">
+        <v>460</v>
+      </c>
+      <c r="C237">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
+      <c r="A238">
+        <v>952</v>
+      </c>
+      <c r="B238">
+        <v>470</v>
+      </c>
+      <c r="C238">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3">
+      <c r="A239">
+        <v>951</v>
+      </c>
+      <c r="B239">
+        <v>480</v>
+      </c>
+      <c r="C239">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3">
+      <c r="A240">
+        <v>951</v>
+      </c>
+      <c r="B240">
+        <v>490</v>
+      </c>
+      <c r="C240">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3">
+      <c r="A241">
+        <v>952</v>
+      </c>
+      <c r="B241">
+        <v>500</v>
+      </c>
+      <c r="C241">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
+      <c r="A242">
+        <v>951</v>
+      </c>
+      <c r="B242">
+        <v>510</v>
+      </c>
+      <c r="C242">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
+      <c r="A243">
+        <v>951</v>
+      </c>
+      <c r="B243">
+        <v>520</v>
+      </c>
+      <c r="C243">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3">
+      <c r="A244">
+        <v>951</v>
+      </c>
+      <c r="B244">
+        <v>530</v>
+      </c>
+      <c r="C244">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3">
+      <c r="A245">
+        <v>951</v>
+      </c>
+      <c r="B245">
+        <v>540</v>
+      </c>
+      <c r="C245">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3">
+      <c r="A246">
+        <v>951</v>
+      </c>
+      <c r="B246">
+        <v>550</v>
+      </c>
+      <c r="C246">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
+      <c r="A247">
+        <v>951</v>
+      </c>
+      <c r="B247">
+        <v>560</v>
+      </c>
+      <c r="C247">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248">
+        <v>951</v>
+      </c>
+      <c r="B248">
+        <v>570</v>
+      </c>
+      <c r="C248">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3">
+      <c r="A249">
+        <v>951</v>
+      </c>
+      <c r="B249">
+        <v>580</v>
+      </c>
+      <c r="C249">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3">
+      <c r="A250">
+        <v>951</v>
+      </c>
+      <c r="B250">
+        <v>590</v>
+      </c>
+      <c r="C250">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3">
+      <c r="A251">
+        <v>951</v>
+      </c>
+      <c r="B251">
+        <v>600</v>
+      </c>
+      <c r="C251">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="A252">
+        <v>950</v>
+      </c>
+      <c r="B252">
+        <v>610</v>
+      </c>
+      <c r="C252">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3">
+      <c r="A253">
+        <v>951</v>
+      </c>
+      <c r="B253">
+        <v>620</v>
+      </c>
+      <c r="C253">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254">
+        <v>951</v>
+      </c>
+      <c r="B254">
+        <v>630</v>
+      </c>
+      <c r="C254">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3">
+      <c r="A255">
+        <v>951</v>
+      </c>
+      <c r="B255">
+        <v>640</v>
+      </c>
+      <c r="C255">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3">
+      <c r="A256">
+        <v>951</v>
+      </c>
+      <c r="B256">
+        <v>650</v>
+      </c>
+      <c r="C256">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
+      <c r="A257">
+        <v>951</v>
+      </c>
+      <c r="B257">
+        <v>660</v>
+      </c>
+      <c r="C257">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3">
+      <c r="A258">
+        <v>950</v>
+      </c>
+      <c r="B258">
+        <v>670</v>
+      </c>
+      <c r="C258">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3">
+      <c r="A259">
+        <v>951</v>
+      </c>
+      <c r="B259">
+        <v>680</v>
+      </c>
+      <c r="C259">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3">
+      <c r="A260">
+        <v>950</v>
+      </c>
+      <c r="B260">
+        <v>690</v>
+      </c>
+      <c r="C260">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3">
+      <c r="A261">
+        <v>951</v>
+      </c>
+      <c r="B261">
+        <v>700</v>
+      </c>
+      <c r="C261">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3">
+      <c r="A262">
+        <v>951</v>
+      </c>
+      <c r="B262">
+        <v>710</v>
+      </c>
+      <c r="C262">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3">
+      <c r="A263">
+        <v>951</v>
+      </c>
+      <c r="B263">
+        <v>720</v>
+      </c>
+      <c r="C263">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3">
+      <c r="A264">
+        <v>951</v>
+      </c>
+      <c r="B264">
+        <v>730</v>
+      </c>
+      <c r="C264">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3">
+      <c r="A265">
+        <v>951</v>
+      </c>
+      <c r="B265">
+        <v>740</v>
+      </c>
+      <c r="C265">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3">
+      <c r="A266">
+        <v>950</v>
+      </c>
+      <c r="B266">
+        <v>750</v>
+      </c>
+      <c r="C266">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3">
+      <c r="A267">
+        <v>950</v>
+      </c>
+      <c r="B267">
+        <v>760</v>
+      </c>
+      <c r="C267">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3">
+      <c r="A268">
+        <v>951</v>
+      </c>
+      <c r="B268">
+        <v>770</v>
+      </c>
+      <c r="C268">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3">
+      <c r="A269">
+        <v>950</v>
+      </c>
+      <c r="B269">
+        <v>780</v>
+      </c>
+      <c r="C269">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3">
+      <c r="A270">
+        <v>951</v>
+      </c>
+      <c r="B270">
+        <v>790</v>
+      </c>
+      <c r="C270">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3">
+      <c r="A271">
+        <v>951</v>
+      </c>
+      <c r="B271">
+        <v>800</v>
+      </c>
+      <c r="C271">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3">
+      <c r="A272">
+        <v>950</v>
+      </c>
+      <c r="B272">
+        <v>810</v>
+      </c>
+      <c r="C272">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273">
+        <v>950</v>
+      </c>
+      <c r="B273">
+        <v>820</v>
+      </c>
+      <c r="C273">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="A274">
+        <v>950</v>
+      </c>
+      <c r="B274">
+        <v>830</v>
+      </c>
+      <c r="C274">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3">
+      <c r="A275">
+        <v>951</v>
+      </c>
+      <c r="B275">
+        <v>840</v>
+      </c>
+      <c r="C275">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276">
+        <v>950</v>
+      </c>
+      <c r="B276">
+        <v>850</v>
+      </c>
+      <c r="C276">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3">
+      <c r="A277">
+        <v>950</v>
+      </c>
+      <c r="B277">
+        <v>860</v>
+      </c>
+      <c r="C277">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3">
+      <c r="A278">
+        <v>950</v>
+      </c>
+      <c r="B278">
+        <v>870</v>
+      </c>
+      <c r="C278">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3">
+      <c r="A279">
+        <v>949</v>
+      </c>
+      <c r="B279">
+        <v>880</v>
+      </c>
+      <c r="C279">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3">
+      <c r="A280">
+        <v>950</v>
+      </c>
+      <c r="B280">
+        <v>890</v>
+      </c>
+      <c r="C280">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3">
+      <c r="A281">
+        <v>949</v>
+      </c>
+      <c r="B281">
+        <v>900</v>
+      </c>
+      <c r="C281">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3">
+      <c r="A282">
+        <v>950</v>
+      </c>
+      <c r="B282">
+        <v>910</v>
+      </c>
+      <c r="C282">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3">
+      <c r="A283">
+        <v>950</v>
+      </c>
+      <c r="B283">
+        <v>920</v>
+      </c>
+      <c r="C283">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3">
+      <c r="A284">
+        <v>949</v>
+      </c>
+      <c r="B284">
+        <v>930</v>
+      </c>
+      <c r="C284">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3">
+      <c r="A285">
+        <v>950</v>
+      </c>
+      <c r="B285">
+        <v>940</v>
+      </c>
+      <c r="C285">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3">
+      <c r="A286">
+        <v>950</v>
+      </c>
+      <c r="B286">
+        <v>950</v>
+      </c>
+      <c r="C286">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3">
+      <c r="A287">
+        <v>950</v>
+      </c>
+      <c r="B287">
+        <v>960</v>
+      </c>
+      <c r="C287">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>